<commit_message>
docs(flag): add coronavirus / Covid-19 flag code
</commit_message>
<xml_diff>
--- a/docs/ydh_alert_list.xlsx
+++ b/docs/ydh_alert_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9348" windowHeight="2676"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9345" windowHeight="2670"/>
   </bookViews>
   <sheets>
     <sheet name="ydh_alert_list" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="228">
   <si>
     <t>Legacy Alert and/or Allergy Information</t>
   </si>
@@ -694,13 +694,22 @@
   </si>
   <si>
     <t>SNOMED_Display</t>
+  </si>
+  <si>
+    <t>WN-CoV</t>
+  </si>
+  <si>
+    <t>WN-Cov swab taken</t>
+  </si>
+  <si>
+    <t>Patient swabbed for coronavirus / Covid-19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -833,6 +842,12 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1177,13 +1192,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1325,8 +1342,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E83" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E83"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E84" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E84"/>
   <tableColumns count="5">
     <tableColumn id="6" name="YDH_TrakCare_Code" dataDxfId="4"/>
     <tableColumn id="1" name="YDH_TrakCare_Display" dataDxfId="3"/>
@@ -1601,23 +1618,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="131.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="83.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="83.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="131.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="83.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>221</v>
       </c>
@@ -1634,7 +1651,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1645,7 +1662,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1660,7 +1677,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1675,7 +1692,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1690,7 +1707,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1705,7 +1722,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1720,7 +1737,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1735,7 +1752,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1750,7 +1767,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1765,7 +1782,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -1780,7 +1797,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1791,7 +1808,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1802,7 +1819,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1817,7 +1834,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -1832,7 +1849,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1843,7 +1860,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -1856,7 +1873,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
@@ -1869,7 +1886,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -1884,7 +1901,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1899,7 +1916,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
@@ -1914,7 +1931,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -1929,7 +1946,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -1944,7 +1961,7 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1959,7 +1976,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1974,7 +1991,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -1989,7 +2006,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -2004,7 +2021,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -2015,7 +2032,7 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -2026,7 +2043,7 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
@@ -2039,7 +2056,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -2054,7 +2071,7 @@
       </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>59</v>
       </c>
@@ -2069,7 +2086,7 @@
       </c>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -2084,7 +2101,7 @@
       </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>63</v>
       </c>
@@ -2099,7 +2116,7 @@
       </c>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>65</v>
       </c>
@@ -2114,7 +2131,7 @@
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>67</v>
       </c>
@@ -2129,7 +2146,7 @@
       </c>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>69</v>
       </c>
@@ -2144,7 +2161,7 @@
       </c>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>71</v>
       </c>
@@ -2159,7 +2176,7 @@
       </c>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
@@ -2174,7 +2191,7 @@
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>75</v>
       </c>
@@ -2185,7 +2202,7 @@
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>76</v>
       </c>
@@ -2200,7 +2217,7 @@
       </c>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>78</v>
       </c>
@@ -2215,7 +2232,7 @@
       </c>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>80</v>
       </c>
@@ -2230,7 +2247,7 @@
       </c>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>82</v>
       </c>
@@ -2245,7 +2262,7 @@
       </c>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
@@ -2256,7 +2273,7 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>86</v>
       </c>
@@ -2271,7 +2288,7 @@
       </c>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>88</v>
       </c>
@@ -2286,7 +2303,7 @@
       </c>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>90</v>
       </c>
@@ -2301,7 +2318,7 @@
       </c>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
@@ -2316,7 +2333,7 @@
       </c>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>94</v>
       </c>
@@ -2331,7 +2348,7 @@
       </c>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>96</v>
       </c>
@@ -2346,7 +2363,7 @@
       </c>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>98</v>
       </c>
@@ -2357,7 +2374,7 @@
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>100</v>
       </c>
@@ -2372,7 +2389,7 @@
       </c>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>102</v>
       </c>
@@ -2383,7 +2400,7 @@
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>104</v>
       </c>
@@ -2398,7 +2415,7 @@
       </c>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>106</v>
       </c>
@@ -2413,7 +2430,7 @@
       </c>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>108</v>
       </c>
@@ -2428,7 +2445,7 @@
       </c>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>110</v>
       </c>
@@ -2439,7 +2456,7 @@
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>112</v>
       </c>
@@ -2454,7 +2471,7 @@
       </c>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>114</v>
       </c>
@@ -2469,7 +2486,7 @@
       </c>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>116</v>
       </c>
@@ -2484,7 +2501,7 @@
       </c>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>118</v>
       </c>
@@ -2499,7 +2516,7 @@
       </c>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>120</v>
       </c>
@@ -2514,7 +2531,7 @@
       </c>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>122</v>
       </c>
@@ -2525,7 +2542,7 @@
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>124</v>
       </c>
@@ -2540,7 +2557,7 @@
       </c>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>126</v>
       </c>
@@ -2551,7 +2568,7 @@
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>128</v>
       </c>
@@ -2564,7 +2581,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>130</v>
       </c>
@@ -2579,7 +2596,7 @@
       </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>132</v>
       </c>
@@ -2594,7 +2611,7 @@
       </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>134</v>
       </c>
@@ -2609,7 +2626,7 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>136</v>
       </c>
@@ -2624,7 +2641,7 @@
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>138</v>
       </c>
@@ -2635,7 +2652,7 @@
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>140</v>
       </c>
@@ -2650,7 +2667,7 @@
       </c>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>142</v>
       </c>
@@ -2665,7 +2682,7 @@
       </c>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>144</v>
       </c>
@@ -2676,7 +2693,7 @@
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>146</v>
       </c>
@@ -2687,7 +2704,7 @@
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>148</v>
       </c>
@@ -2702,7 +2719,7 @@
       </c>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>150</v>
       </c>
@@ -2717,7 +2734,7 @@
       </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>152</v>
       </c>
@@ -2728,7 +2745,7 @@
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>154</v>
       </c>
@@ -2739,7 +2756,7 @@
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>156</v>
       </c>
@@ -2750,7 +2767,7 @@
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>158</v>
       </c>
@@ -2765,16 +2782,29 @@
       </c>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C83" s="7"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C83" s="5"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
docs(flag): update covid-19 entries
</commit_message>
<xml_diff>
--- a/docs/ydh_alert_list.xlsx
+++ b/docs/ydh_alert_list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frazer.smith\Documents\Projects\ydh-fhir-listeners\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frazer.smith\Documents\Projects\public\ydh-fhir-listeners\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9345" windowHeight="2670"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9348" windowHeight="2676"/>
   </bookViews>
   <sheets>
     <sheet name="ydh_alert_list" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="234">
   <si>
     <t>Legacy Alert and/or Allergy Information</t>
   </si>
@@ -699,10 +699,28 @@
     <t>WN-CoV</t>
   </si>
   <si>
-    <t>WN-Cov swab taken</t>
-  </si>
-  <si>
     <t>Patient swabbed for coronavirus / Covid-19</t>
+  </si>
+  <si>
+    <t>WN-CoV: Pending - Swab Taken</t>
+  </si>
+  <si>
+    <t>WIN-CoV-Negative</t>
+  </si>
+  <si>
+    <t>WIN-CoV-Positive</t>
+  </si>
+  <si>
+    <t>WN-CoV: Positive</t>
+  </si>
+  <si>
+    <t>WN-CoV: Negative</t>
+  </si>
+  <si>
+    <t>COVID-19</t>
+  </si>
+  <si>
+    <t>Suspected COVID-19</t>
   </si>
 </sst>
 </file>
@@ -1342,8 +1360,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E84" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E86" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E86"/>
   <tableColumns count="5">
     <tableColumn id="6" name="YDH_TrakCare_Code" dataDxfId="4"/>
     <tableColumn id="1" name="YDH_TrakCare_Display" dataDxfId="3"/>
@@ -1618,23 +1636,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="C68" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="131.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="83.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="83.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="131.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="83.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>221</v>
       </c>
@@ -1651,7 +1669,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1662,7 +1680,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1677,7 +1695,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1692,7 +1710,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1707,7 +1725,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1722,7 +1740,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1737,7 +1755,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1752,7 +1770,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1767,7 +1785,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1782,7 +1800,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -1797,7 +1815,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1808,7 +1826,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1819,7 +1837,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1834,7 +1852,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -1849,7 +1867,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1860,7 +1878,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -1873,7 +1891,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
@@ -1886,7 +1904,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -1901,7 +1919,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1916,7 +1934,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
@@ -1931,7 +1949,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -1946,7 +1964,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -1961,7 +1979,7 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1976,7 +1994,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1991,7 +2009,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -2006,7 +2024,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -2021,7 +2039,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -2032,7 +2050,7 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -2043,7 +2061,7 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
@@ -2056,7 +2074,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -2071,7 +2089,7 @@
       </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>59</v>
       </c>
@@ -2086,7 +2104,7 @@
       </c>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -2101,7 +2119,7 @@
       </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>63</v>
       </c>
@@ -2116,7 +2134,7 @@
       </c>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>65</v>
       </c>
@@ -2131,7 +2149,7 @@
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>67</v>
       </c>
@@ -2146,7 +2164,7 @@
       </c>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>69</v>
       </c>
@@ -2161,7 +2179,7 @@
       </c>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>71</v>
       </c>
@@ -2176,7 +2194,7 @@
       </c>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
@@ -2191,7 +2209,7 @@
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>75</v>
       </c>
@@ -2202,7 +2220,7 @@
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>76</v>
       </c>
@@ -2217,7 +2235,7 @@
       </c>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>78</v>
       </c>
@@ -2232,7 +2250,7 @@
       </c>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>80</v>
       </c>
@@ -2247,7 +2265,7 @@
       </c>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>82</v>
       </c>
@@ -2262,7 +2280,7 @@
       </c>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
@@ -2273,7 +2291,7 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>86</v>
       </c>
@@ -2288,7 +2306,7 @@
       </c>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>88</v>
       </c>
@@ -2303,7 +2321,7 @@
       </c>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>90</v>
       </c>
@@ -2318,7 +2336,7 @@
       </c>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
@@ -2333,7 +2351,7 @@
       </c>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>94</v>
       </c>
@@ -2348,7 +2366,7 @@
       </c>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>96</v>
       </c>
@@ -2363,7 +2381,7 @@
       </c>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>98</v>
       </c>
@@ -2374,7 +2392,7 @@
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>100</v>
       </c>
@@ -2389,7 +2407,7 @@
       </c>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>102</v>
       </c>
@@ -2400,7 +2418,7 @@
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>104</v>
       </c>
@@ -2415,7 +2433,7 @@
       </c>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>106</v>
       </c>
@@ -2430,7 +2448,7 @@
       </c>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>108</v>
       </c>
@@ -2445,7 +2463,7 @@
       </c>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>110</v>
       </c>
@@ -2456,7 +2474,7 @@
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>112</v>
       </c>
@@ -2471,7 +2489,7 @@
       </c>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>114</v>
       </c>
@@ -2486,7 +2504,7 @@
       </c>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>116</v>
       </c>
@@ -2501,7 +2519,7 @@
       </c>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>118</v>
       </c>
@@ -2516,7 +2534,7 @@
       </c>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>120</v>
       </c>
@@ -2531,7 +2549,7 @@
       </c>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>122</v>
       </c>
@@ -2542,7 +2560,7 @@
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>124</v>
       </c>
@@ -2557,7 +2575,7 @@
       </c>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>126</v>
       </c>
@@ -2568,7 +2586,7 @@
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>128</v>
       </c>
@@ -2581,7 +2599,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>130</v>
       </c>
@@ -2596,7 +2614,7 @@
       </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>132</v>
       </c>
@@ -2611,7 +2629,7 @@
       </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>134</v>
       </c>
@@ -2626,7 +2644,7 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>136</v>
       </c>
@@ -2641,7 +2659,7 @@
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>138</v>
       </c>
@@ -2652,7 +2670,7 @@
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>140</v>
       </c>
@@ -2667,7 +2685,7 @@
       </c>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>142</v>
       </c>
@@ -2682,7 +2700,7 @@
       </c>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>144</v>
       </c>
@@ -2693,7 +2711,7 @@
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>146</v>
       </c>
@@ -2704,7 +2722,7 @@
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>148</v>
       </c>
@@ -2719,7 +2737,7 @@
       </c>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>150</v>
       </c>
@@ -2734,7 +2752,7 @@
       </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>152</v>
       </c>
@@ -2745,7 +2763,7 @@
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>154</v>
       </c>
@@ -2756,7 +2774,7 @@
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>156</v>
       </c>
@@ -2767,7 +2785,7 @@
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>158</v>
       </c>
@@ -2782,29 +2800,59 @@
       </c>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="B83" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C83" s="7">
+        <v>840544004</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E83" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C83" s="7"/>
-      <c r="D83" s="6"/>
-      <c r="E83" s="6" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C84" s="3"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C85" s="3">
+        <v>840539006</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C84" s="5"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>